<commit_message>
configuracion eigrpv6 y ospf multiarea
</commit_message>
<xml_diff>
--- a/docs/masks.xlsx
+++ b/docs/masks.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna3-lx20\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC53BF53-A167-49F9-8806-2B937FF51578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D2795C-0ACB-4EBB-A5B3-1C6EBC09815F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="1" xr2:uid="{36AD6682-3937-4C44-9F39-CDC474161464}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="2" xr2:uid="{36AD6682-3937-4C44-9F39-CDC474161464}"/>
   </bookViews>
   <sheets>
     <sheet name="AND" sheetId="1" r:id="rId1"/>
     <sheet name="WILDCARD" sheetId="2" r:id="rId2"/>
+    <sheet name="IPv4" sheetId="4" r:id="rId3"/>
+    <sheet name="IPv6" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="104">
   <si>
     <t>IP</t>
   </si>
@@ -162,13 +164,641 @@
   </si>
   <si>
     <t>00010100</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>LINK-LOCAL</t>
+  </si>
+  <si>
+    <t>UNIQUE-LOCAL</t>
+  </si>
+  <si>
+    <t>GLOBAL UNIQUE</t>
+  </si>
+  <si>
+    <t>MULTICAST</t>
+  </si>
+  <si>
+    <t>INI BIN</t>
+  </si>
+  <si>
+    <t>INI DEC</t>
+  </si>
+  <si>
+    <t>FIN BIN</t>
+  </si>
+  <si>
+    <t>FIN DEC</t>
+  </si>
+  <si>
+    <t>RANGO PUBLICO</t>
+  </si>
+  <si>
+    <t>RANGO PRIVADO</t>
+  </si>
+  <si>
+    <t>CLASE</t>
+  </si>
+  <si>
+    <t>IPv4</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>0.0.0.0</t>
+  </si>
+  <si>
+    <t>128.0.0.0</t>
+  </si>
+  <si>
+    <t>192.0.0.0</t>
+  </si>
+  <si>
+    <t>224.0.0.0</t>
+  </si>
+  <si>
+    <t>240.0.0.0</t>
+  </si>
+  <si>
+    <t>Multicast</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>10.0.0.0</t>
+  </si>
+  <si>
+    <t>172.16.0.0</t>
+  </si>
+  <si>
+    <t>172.31.255.255</t>
+  </si>
+  <si>
+    <t>192.168.0.0</t>
+  </si>
+  <si>
+    <t>10101100.
+00010000</t>
+  </si>
+  <si>
+    <t>10101100.
+00011111</t>
+  </si>
+  <si>
+    <t>11000000.
+10101000.
+00000000</t>
+  </si>
+  <si>
+    <t>11000000.
+10101000.
+11111111</t>
+  </si>
+  <si>
+    <t>INI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIN </t>
+  </si>
+  <si>
+    <t>SECUENCIA</t>
+  </si>
+  <si>
+    <t>BITS</t>
+  </si>
+  <si>
+    <t>Equivalencia</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>000::</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.0000.0000.0000</t>
+    </r>
+  </si>
+  <si>
+    <t>IPv4 Publico</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1111.110</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.0000.0000</t>
+    </r>
+  </si>
+  <si>
+    <t>IPv4 Privado</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00::</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1111.1110.10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00.0000</t>
+    </r>
+  </si>
+  <si>
+    <t>IPv4 A.P.I.P.A.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FE8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0::</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1111.1111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0000.0000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00::</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FF::</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FEB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>F::</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FF::</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FFF::</t>
+    </r>
+  </si>
+  <si>
+    <t>IPv4 Multicast</t>
+  </si>
+  <si>
+    <t>INI BIN2</t>
+  </si>
+  <si>
+    <t>INI DEC3</t>
+  </si>
+  <si>
+    <t>FIN BIN4</t>
+  </si>
+  <si>
+    <t>FIN DEC5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0000000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1111111</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>111111</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>110</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>110</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>11111</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1110</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1110</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1111</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1111</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,16 +819,70 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -206,11 +890,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -219,13 +921,92 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -250,6 +1031,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -265,7 +1047,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -300,13 +1081,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4E595DD-EE7A-49BC-8F0D-AFA4A15B4418}" name="Tabla2" displayName="Tabla2" ref="G1:J5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4E595DD-EE7A-49BC-8F0D-AFA4A15B4418}" name="Tabla2" displayName="Tabla2" ref="G1:J5" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="G1:J5" xr:uid="{A4E595DD-EE7A-49BC-8F0D-AFA4A15B4418}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3A913605-BDEA-42BC-9394-976D1A61F6F3}" name="Octeto 1" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{0E0F1899-3D48-4D56-B0A2-54B85E90D0AA}" name="Octeto 2" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{CFB38C83-BDB5-41C0-93C5-7B5A510B9C29}" name="Octeto 3" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{C868478B-C494-4599-A894-E9E0EA94429F}" name="Octeto 4" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{3A913605-BDEA-42BC-9394-976D1A61F6F3}" name="Octeto 1" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{0E0F1899-3D48-4D56-B0A2-54B85E90D0AA}" name="Octeto 2" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{CFB38C83-BDB5-41C0-93C5-7B5A510B9C29}" name="Octeto 3" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{C868478B-C494-4599-A894-E9E0EA94429F}" name="Octeto 4" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -327,15 +1108,30 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C524E3DC-741B-49B2-BD82-FCE57ED61A4F}" name="Tabla25" displayName="Tabla25" ref="G1:J5" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C524E3DC-741B-49B2-BD82-FCE57ED61A4F}" name="Tabla25" displayName="Tabla25" ref="G1:J5" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="G1:J5" xr:uid="{C524E3DC-741B-49B2-BD82-FCE57ED61A4F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{900494D8-484D-40C1-86A0-3DF44650F322}" name="Octeto 1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{465010BE-225D-4E63-8A9F-DDFE500E1086}" name="Octeto 2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{C6B84349-35B7-4DEF-A738-34567F9F07FF}" name="Octeto 3" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{777DE849-E293-4EE0-85B5-C3944DEF845E}" name="Octeto 4" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{900494D8-484D-40C1-86A0-3DF44650F322}" name="Octeto 1" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{465010BE-225D-4E63-8A9F-DDFE500E1086}" name="Octeto 2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{C6B84349-35B7-4DEF-A738-34567F9F07FF}" name="Octeto 3" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{777DE849-E293-4EE0-85B5-C3944DEF845E}" name="Octeto 4" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{33D54A2B-5924-481E-B272-30F590824005}" name="Tabla5" displayName="Tabla5" ref="A1:F5" totalsRowShown="0">
+  <autoFilter ref="A1:F5" xr:uid="{33D54A2B-5924-481E-B272-30F590824005}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{97CBED28-5E66-468C-9E87-BE8D686B7A9C}" name="TIPO"/>
+    <tableColumn id="2" xr3:uid="{D9B798F0-6BAA-4635-962F-1FE28C35B2AC}" name="INI"/>
+    <tableColumn id="3" xr3:uid="{41D6A7FB-9A02-4D36-BF5F-64FDB2F740BC}" name="FIN "/>
+    <tableColumn id="4" xr3:uid="{BAD2A253-C88B-4FFD-999E-4B18EC218630}" name="SECUENCIA" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{44159771-05CC-45AB-9DC3-8E6756588E1F}" name="BITS"/>
+    <tableColumn id="6" xr3:uid="{751E486F-C47A-42F0-AED4-CDBDD1E3B4B0}" name="Equivalencia"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -639,7 +1435,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:J5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +1628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F9193A5-56D3-4B37-AF9D-F917C49587E2}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1013,4 +1809,342 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AD1F17-6647-4E86-8909-A1733D780981}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="25" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+    </row>
+    <row r="2" spans="1:9" s="25" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="7">
+        <v>127255255255</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="7">
+        <v>10255255255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="10">
+        <v>191255255255</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="14">
+        <v>223255255255</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="14">
+        <v>192168255255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="10">
+        <v>239255255255</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="19">
+        <v>255255255255</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA3BA68-2579-4503-BBC8-96AFAD838155}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
configuracion ospf multiarea y frame-relay
</commit_message>
<xml_diff>
--- a/docs/masks.xlsx
+++ b/docs/masks.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna3-lx20\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D2795C-0ACB-4EBB-A5B3-1C6EBC09815F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875858C5-D38F-4022-8737-31DA2A3E0D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="2" xr2:uid="{36AD6682-3937-4C44-9F39-CDC474161464}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="4" xr2:uid="{36AD6682-3937-4C44-9F39-CDC474161464}"/>
   </bookViews>
   <sheets>
     <sheet name="AND" sheetId="1" r:id="rId1"/>
     <sheet name="WILDCARD" sheetId="2" r:id="rId2"/>
     <sheet name="IPv4" sheetId="4" r:id="rId3"/>
     <sheet name="IPv6" sheetId="3" r:id="rId4"/>
+    <sheet name="SISTEMAS" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="121">
   <si>
     <t>IP</t>
   </si>
@@ -792,6 +793,57 @@
       </rPr>
       <t>1111</t>
     </r>
+  </si>
+  <si>
+    <t>2^7</t>
+  </si>
+  <si>
+    <t>2^1</t>
+  </si>
+  <si>
+    <t>2^0</t>
+  </si>
+  <si>
+    <t>2^6</t>
+  </si>
+  <si>
+    <t>2^5</t>
+  </si>
+  <si>
+    <t>2^4</t>
+  </si>
+  <si>
+    <t>2^3</t>
+  </si>
+  <si>
+    <t>2^2</t>
+  </si>
+  <si>
+    <t>10^3</t>
+  </si>
+  <si>
+    <t>10^2</t>
+  </si>
+  <si>
+    <t>10^1</t>
+  </si>
+  <si>
+    <t>10^0</t>
+  </si>
+  <si>
+    <t>16^3</t>
+  </si>
+  <si>
+    <t>16^2</t>
+  </si>
+  <si>
+    <t>16^1</t>
+  </si>
+  <si>
+    <t>16^0</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -882,7 +934,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -908,11 +960,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -957,9 +1089,6 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -967,9 +1096,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -977,9 +1103,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -997,13 +1120,135 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="35">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1081,13 +1326,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4E595DD-EE7A-49BC-8F0D-AFA4A15B4418}" name="Tabla2" displayName="Tabla2" ref="G1:J5" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4E595DD-EE7A-49BC-8F0D-AFA4A15B4418}" name="Tabla2" displayName="Tabla2" ref="G1:J5" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="G1:J5" xr:uid="{A4E595DD-EE7A-49BC-8F0D-AFA4A15B4418}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3A913605-BDEA-42BC-9394-976D1A61F6F3}" name="Octeto 1" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{0E0F1899-3D48-4D56-B0A2-54B85E90D0AA}" name="Octeto 2" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{CFB38C83-BDB5-41C0-93C5-7B5A510B9C29}" name="Octeto 3" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{C868478B-C494-4599-A894-E9E0EA94429F}" name="Octeto 4" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{3A913605-BDEA-42BC-9394-976D1A61F6F3}" name="Octeto 1" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{0E0F1899-3D48-4D56-B0A2-54B85E90D0AA}" name="Octeto 2" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{CFB38C83-BDB5-41C0-93C5-7B5A510B9C29}" name="Octeto 3" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{C868478B-C494-4599-A894-E9E0EA94429F}" name="Octeto 4" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1108,13 +1353,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C524E3DC-741B-49B2-BD82-FCE57ED61A4F}" name="Tabla25" displayName="Tabla25" ref="G1:J5" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C524E3DC-741B-49B2-BD82-FCE57ED61A4F}" name="Tabla25" displayName="Tabla25" ref="G1:J5" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="G1:J5" xr:uid="{C524E3DC-741B-49B2-BD82-FCE57ED61A4F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{900494D8-484D-40C1-86A0-3DF44650F322}" name="Octeto 1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{465010BE-225D-4E63-8A9F-DDFE500E1086}" name="Octeto 2" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{C6B84349-35B7-4DEF-A738-34567F9F07FF}" name="Octeto 3" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{777DE849-E293-4EE0-85B5-C3944DEF845E}" name="Octeto 4" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{900494D8-484D-40C1-86A0-3DF44650F322}" name="Octeto 1" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{465010BE-225D-4E63-8A9F-DDFE500E1086}" name="Octeto 2" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{C6B84349-35B7-4DEF-A738-34567F9F07FF}" name="Octeto 3" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{777DE849-E293-4EE0-85B5-C3944DEF845E}" name="Octeto 4" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1127,9 +1372,52 @@
     <tableColumn id="1" xr3:uid="{97CBED28-5E66-468C-9E87-BE8D686B7A9C}" name="TIPO"/>
     <tableColumn id="2" xr3:uid="{D9B798F0-6BAA-4635-962F-1FE28C35B2AC}" name="INI"/>
     <tableColumn id="3" xr3:uid="{41D6A7FB-9A02-4D36-BF5F-64FDB2F740BC}" name="FIN "/>
-    <tableColumn id="4" xr3:uid="{BAD2A253-C88B-4FFD-999E-4B18EC218630}" name="SECUENCIA" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{BAD2A253-C88B-4FFD-999E-4B18EC218630}" name="SECUENCIA" dataDxfId="22"/>
     <tableColumn id="5" xr3:uid="{44159771-05CC-45AB-9DC3-8E6756588E1F}" name="BITS"/>
     <tableColumn id="6" xr3:uid="{751E486F-C47A-42F0-AED4-CDBDD1E3B4B0}" name="Equivalencia"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{241CEDEC-CD85-4906-A964-ADD497FA1B71}" name="Tabla6" displayName="Tabla6" ref="F1:M3" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="F1:M3" xr:uid="{241CEDEC-CD85-4906-A964-ADD497FA1B71}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{D4E7EDB8-FF1D-4F29-B7DD-2EDE3DC55F5B}" name="2^7" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{D4B53AA7-C8A4-4444-A806-522A1E98209A}" name="2^6" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{1A4F6D5A-23A1-4BC4-B0F9-E41813BC6D3D}" name="2^5" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{AE635144-43B6-49B9-BA3A-3CB9EFE18E7D}" name="2^4" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{EE4BA23C-1665-4E54-8F63-625BCCF375D2}" name="2^3" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{80113BAB-9342-469F-95E0-91BB252846C2}" name="2^2" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{DA9E03E8-AF39-4533-864C-F4A41C0B2DFC}" name="2^1" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{3E8E00B5-EF9C-4889-AA31-469C83886640}" name="2^0" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A0ADC668-A62D-4A5A-852F-EC8FD6B6C139}" name="Tabla69" displayName="Tabla69" ref="O1:R3" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="O1:R3" xr:uid="{A0ADC668-A62D-4A5A-852F-EC8FD6B6C139}"/>
+  <tableColumns count="4">
+    <tableColumn id="5" xr3:uid="{3EF44B2F-BBB5-4C44-A661-E3525266F154}" name="16^3" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{652D1B64-6962-475B-86D0-4855764E5F35}" name="16^2" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{C2BCFC9B-049A-4EEE-BE1A-A627D8C9C6A3}" name="16^1" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{5D06ABA4-E949-4C18-A2D9-F28AED245775}" name="16^0" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{796CE725-D254-4AFD-9CA3-A53DD6BA0736}" name="Tabla6811" displayName="Tabla6811" ref="A1:D3" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:D3" xr:uid="{796CE725-D254-4AFD-9CA3-A53DD6BA0736}"/>
+  <tableColumns count="4">
+    <tableColumn id="5" xr3:uid="{CD16CCF4-5C68-48AF-A455-B1B9AC09ED5A}" name="10^3" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{67F18D92-FF52-4E8B-A582-32DB2F26FB71}" name="10^2" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{01D264AC-510C-49E9-8469-4AA6C6C00AE1}" name="10^1" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{8A0282F9-0D07-4F6D-B983-F01EFC91EAC5}" name="10^0" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1815,71 +2103,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AD1F17-6647-4E86-8909-A1733D780981}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="22" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="21" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="19" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="19" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="25" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:9" s="22" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-    </row>
-    <row r="2" spans="1:9" s="25" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+    </row>
+    <row r="2" spans="1:9" s="22" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="23" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="25" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1908,7 +2196,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="26" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1937,7 +2225,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="36.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="27" t="s">
         <v>51</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -1966,7 +2254,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="26" t="s">
         <v>52</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1981,35 +2269,35 @@
       <c r="E6" s="10">
         <v>239255255255</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="18">
         <v>255255255255</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2147,4 +2435,178 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7944B7DB-DF92-4A1D-BDE5-8D0D528A6BF0}">
+  <dimension ref="A1:R3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="18" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="3">
+        <v>100</v>
+      </c>
+      <c r="C2" s="3">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="35">
+        <v>128</v>
+      </c>
+      <c r="G2" s="36">
+        <v>64</v>
+      </c>
+      <c r="H2" s="36">
+        <v>32</v>
+      </c>
+      <c r="I2" s="37">
+        <v>16</v>
+      </c>
+      <c r="J2" s="3">
+        <v>8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>4</v>
+      </c>
+      <c r="L2" s="3">
+        <v>2</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1</v>
+      </c>
+      <c r="O2" s="3">
+        <v>4096</v>
+      </c>
+      <c r="P2" s="3">
+        <v>256</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>16</v>
+      </c>
+      <c r="R2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="38">
+        <v>1</v>
+      </c>
+      <c r="G3" s="39">
+        <v>0</v>
+      </c>
+      <c r="H3" s="39">
+        <v>1</v>
+      </c>
+      <c r="I3" s="40">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="3">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>